<commit_message>
added dob for login
</commit_message>
<xml_diff>
--- a/public/templates/student-upload-template.xlsx
+++ b/public/templates/student-upload-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,13 +406,14 @@
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -429,24 +430,27 @@
         <v>Phone</v>
       </c>
       <c r="E1" t="str">
+        <v>DOB</v>
+      </c>
+      <c r="F1" t="str">
         <v>Semester</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Course</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Shift</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Section</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Reg. No.</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Roll No.</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>ABC Id</v>
       </c>
     </row>
@@ -464,24 +468,27 @@
         <v>9876543210</v>
       </c>
       <c r="E2" t="str">
+        <v>01-01-1998</v>
+      </c>
+      <c r="F2" t="str">
         <v>3</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>B.Tech Computer Science</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>DAY</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>A</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>REG123456</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>CS123</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>ABC123456</v>
       </c>
     </row>
@@ -499,24 +506,27 @@
         <v>9876543211</v>
       </c>
       <c r="E3" t="str">
+        <v>15-05-1999</v>
+      </c>
+      <c r="F3" t="str">
         <v>5</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>B.Tech Electronics</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>MORNING</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>B</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>REG789012</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <v>EC456</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <v>ABC789012</v>
       </c>
     </row>
@@ -534,30 +544,33 @@
         <v>9876543212</v>
       </c>
       <c r="E4" t="str">
+        <v>23-11-2000</v>
+      </c>
+      <c r="F4" t="str">
         <v>7</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <v>MCA</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>EVENING</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>C</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <v>REG456789</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" t="str">
         <v>MCA789</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <v>ABC456789</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>